<commit_message>
[Updated] - Ajuste de codigo - mayor recursibilidad
</commit_message>
<xml_diff>
--- a/Docs/python/Test_template_Fortinet_Products.xlsx
+++ b/Docs/python/Test_template_Fortinet_Products.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="10"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="FortiGate" sheetId="1" state="visible" r:id="rId3"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="164">
   <si>
     <t xml:space="preserve">UNIT</t>
   </si>
@@ -59,7 +59,7 @@
     <t xml:space="preserve">A2</t>
   </si>
   <si>
-    <t xml:space="preserve">A3</t>
+    <t xml:space="preserve">ME actualize</t>
   </si>
   <si>
     <t xml:space="preserve">A4</t>
@@ -513,6 +513,15 @@
   </si>
   <si>
     <t xml:space="preserve">K14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FortiGate-30G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FG-30G</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 x GE RJ45 ports (including 3 x Internal Ports, 1 x WAN Ports)</t>
   </si>
 </sst>
 </file>
@@ -522,7 +531,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -544,6 +553,19 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -588,12 +610,20 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -791,8 +821,8 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -981,18 +1011,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G8" activeCellId="0" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.02"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="11.96"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="0" width="14.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="66.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="11.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="14.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="14.6"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1062,6 +1094,29 @@
       </c>
       <c r="G3" s="1" t="s">
         <v>160</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>395</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>